<commit_message>
Cambios a tipo de Examen
Cambios al perfil y a los tipos de examenes
</commit_message>
<xml_diff>
--- a/documents/translates.xlsx
+++ b/documents/translates.xlsx
@@ -437,7 +437,7 @@
   <dimension ref="A1:S8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="S8" sqref="J2:S8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -451,16 +451,11 @@
     <col min="7" max="7" width="40.42578125" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="48" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="0" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="33.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="38.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="39.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="49.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="44.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="44.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="42.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="44" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="44.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="49.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="55.28515625" customWidth="1"/>
+    <col min="11" max="12" width="47.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="52.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="18" width="47.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="52.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="30" x14ac:dyDescent="0.25">
@@ -535,7 +530,7 @@
             &lt;/trans-unit&gt;</v>
       </c>
       <c r="I2" s="1" t="str">
-        <f t="shared" ref="I2:S2" si="0">$C$1&amp;I$1&amp;$A2&amp;$D$1&amp;I$1&amp;$A2&amp;$E$1&amp;$B2&amp;$F$1</f>
+        <f t="shared" ref="I2:S8" si="0">$C$1&amp;I$1&amp;$A2&amp;$D$1&amp;I$1&amp;$A2&amp;$E$1&amp;$B2&amp;$F$1</f>
         <v xml:space="preserve">            &lt;trans-unit id="exam_admin"&gt;
                 &lt;source&gt;exam_admin&lt;/source&gt;
                 &lt;target&gt;Administración Examenes &lt;/target&gt;
@@ -627,48 +622,469 @@
             &lt;/trans-unit&gt;</v>
       </c>
       <c r="H3" s="1"/>
+      <c r="J3" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">            &lt;trans-unit id="exam_type"&gt;
+                &lt;source&gt;exam_type&lt;/source&gt;
+                &lt;target&gt;Tipo de Examen&lt;/target&gt;
+            &lt;/trans-unit&gt;</v>
+      </c>
+      <c r="K3" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">            &lt;trans-unit id="title_exam_type"&gt;
+                &lt;source&gt;title_exam_type&lt;/source&gt;
+                &lt;target&gt;Tipo de Examen&lt;/target&gt;
+            &lt;/trans-unit&gt;</v>
+      </c>
+      <c r="L3" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">            &lt;trans-unit id="label_exam_type"&gt;
+                &lt;source&gt;label_exam_type&lt;/source&gt;
+                &lt;target&gt;Tipo de Examen&lt;/target&gt;
+            &lt;/trans-unit&gt;</v>
+      </c>
+      <c r="M3" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">            &lt;trans-unit id="user_form.label_exam_type"&gt;
+                &lt;source&gt;user_form.label_exam_type&lt;/source&gt;
+                &lt;target&gt;Tipo de Examen&lt;/target&gt;
+            &lt;/trans-unit&gt;</v>
+      </c>
+      <c r="N3" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">            &lt;trans-unit id="form.label_exam_type"&gt;
+                &lt;source&gt;form.label_exam_type&lt;/source&gt;
+                &lt;target&gt;Tipo de Examen&lt;/target&gt;
+            &lt;/trans-unit&gt;</v>
+      </c>
+      <c r="O3" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">            &lt;trans-unit id="filter.label_exam_type"&gt;
+                &lt;source&gt;filter.label_exam_type&lt;/source&gt;
+                &lt;target&gt;Tipo de Examen&lt;/target&gt;
+            &lt;/trans-unit&gt;</v>
+      </c>
+      <c r="P3" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">            &lt;trans-unit id="list.label_exam_type"&gt;
+                &lt;source&gt;list.label_exam_type&lt;/source&gt;
+                &lt;target&gt;Tipo de Examen&lt;/target&gt;
+            &lt;/trans-unit&gt;</v>
+      </c>
+      <c r="Q3" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">            &lt;trans-unit id="field.label_exam_type"&gt;
+                &lt;source&gt;field.label_exam_type&lt;/source&gt;
+                &lt;target&gt;Tipo de Examen&lt;/target&gt;
+            &lt;/trans-unit&gt;</v>
+      </c>
+      <c r="R3" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">            &lt;trans-unit id="show.label_exam_type"&gt;
+                &lt;source&gt;show.label_exam_type&lt;/source&gt;
+                &lt;target&gt;Tipo de Examen&lt;/target&gt;
+            &lt;/trans-unit&gt;</v>
+      </c>
+      <c r="S3" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">            &lt;trans-unit id="breadcrumb.link_exam_type"&gt;
+                &lt;source&gt;breadcrumb.link_exam_type&lt;/source&gt;
+                &lt;target&gt;Tipo de Examen&lt;/target&gt;
+            &lt;/trans-unit&gt;</v>
+      </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
       <c r="B4" t="s">
         <v>19</v>
       </c>
+      <c r="J4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">            &lt;trans-unit id="questions"&gt;
+                &lt;source&gt;questions&lt;/source&gt;
+                &lt;target&gt;Preguntas&lt;/target&gt;
+            &lt;/trans-unit&gt;</v>
+      </c>
+      <c r="K4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">            &lt;trans-unit id="title_questions"&gt;
+                &lt;source&gt;title_questions&lt;/source&gt;
+                &lt;target&gt;Preguntas&lt;/target&gt;
+            &lt;/trans-unit&gt;</v>
+      </c>
+      <c r="L4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">            &lt;trans-unit id="label_questions"&gt;
+                &lt;source&gt;label_questions&lt;/source&gt;
+                &lt;target&gt;Preguntas&lt;/target&gt;
+            &lt;/trans-unit&gt;</v>
+      </c>
+      <c r="M4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">            &lt;trans-unit id="user_form.label_questions"&gt;
+                &lt;source&gt;user_form.label_questions&lt;/source&gt;
+                &lt;target&gt;Preguntas&lt;/target&gt;
+            &lt;/trans-unit&gt;</v>
+      </c>
+      <c r="N4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">            &lt;trans-unit id="form.label_questions"&gt;
+                &lt;source&gt;form.label_questions&lt;/source&gt;
+                &lt;target&gt;Preguntas&lt;/target&gt;
+            &lt;/trans-unit&gt;</v>
+      </c>
+      <c r="O4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">            &lt;trans-unit id="filter.label_questions"&gt;
+                &lt;source&gt;filter.label_questions&lt;/source&gt;
+                &lt;target&gt;Preguntas&lt;/target&gt;
+            &lt;/trans-unit&gt;</v>
+      </c>
+      <c r="P4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">            &lt;trans-unit id="list.label_questions"&gt;
+                &lt;source&gt;list.label_questions&lt;/source&gt;
+                &lt;target&gt;Preguntas&lt;/target&gt;
+            &lt;/trans-unit&gt;</v>
+      </c>
+      <c r="Q4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">            &lt;trans-unit id="field.label_questions"&gt;
+                &lt;source&gt;field.label_questions&lt;/source&gt;
+                &lt;target&gt;Preguntas&lt;/target&gt;
+            &lt;/trans-unit&gt;</v>
+      </c>
+      <c r="R4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">            &lt;trans-unit id="show.label_questions"&gt;
+                &lt;source&gt;show.label_questions&lt;/source&gt;
+                &lt;target&gt;Preguntas&lt;/target&gt;
+            &lt;/trans-unit&gt;</v>
+      </c>
+      <c r="S4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">            &lt;trans-unit id="breadcrumb.link_questions"&gt;
+                &lt;source&gt;breadcrumb.link_questions&lt;/source&gt;
+                &lt;target&gt;Preguntas&lt;/target&gt;
+            &lt;/trans-unit&gt;</v>
+      </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>20</v>
       </c>
       <c r="B5" t="s">
         <v>22</v>
       </c>
+      <c r="J5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">            &lt;trans-unit id="answers"&gt;
+                &lt;source&gt;answers&lt;/source&gt;
+                &lt;target&gt;Respuestas&lt;/target&gt;
+            &lt;/trans-unit&gt;</v>
+      </c>
+      <c r="K5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">            &lt;trans-unit id="title_answers"&gt;
+                &lt;source&gt;title_answers&lt;/source&gt;
+                &lt;target&gt;Respuestas&lt;/target&gt;
+            &lt;/trans-unit&gt;</v>
+      </c>
+      <c r="L5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">            &lt;trans-unit id="label_answers"&gt;
+                &lt;source&gt;label_answers&lt;/source&gt;
+                &lt;target&gt;Respuestas&lt;/target&gt;
+            &lt;/trans-unit&gt;</v>
+      </c>
+      <c r="M5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">            &lt;trans-unit id="user_form.label_answers"&gt;
+                &lt;source&gt;user_form.label_answers&lt;/source&gt;
+                &lt;target&gt;Respuestas&lt;/target&gt;
+            &lt;/trans-unit&gt;</v>
+      </c>
+      <c r="N5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">            &lt;trans-unit id="form.label_answers"&gt;
+                &lt;source&gt;form.label_answers&lt;/source&gt;
+                &lt;target&gt;Respuestas&lt;/target&gt;
+            &lt;/trans-unit&gt;</v>
+      </c>
+      <c r="O5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">            &lt;trans-unit id="filter.label_answers"&gt;
+                &lt;source&gt;filter.label_answers&lt;/source&gt;
+                &lt;target&gt;Respuestas&lt;/target&gt;
+            &lt;/trans-unit&gt;</v>
+      </c>
+      <c r="P5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">            &lt;trans-unit id="list.label_answers"&gt;
+                &lt;source&gt;list.label_answers&lt;/source&gt;
+                &lt;target&gt;Respuestas&lt;/target&gt;
+            &lt;/trans-unit&gt;</v>
+      </c>
+      <c r="Q5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">            &lt;trans-unit id="field.label_answers"&gt;
+                &lt;source&gt;field.label_answers&lt;/source&gt;
+                &lt;target&gt;Respuestas&lt;/target&gt;
+            &lt;/trans-unit&gt;</v>
+      </c>
+      <c r="R5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">            &lt;trans-unit id="show.label_answers"&gt;
+                &lt;source&gt;show.label_answers&lt;/source&gt;
+                &lt;target&gt;Respuestas&lt;/target&gt;
+            &lt;/trans-unit&gt;</v>
+      </c>
+      <c r="S5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">            &lt;trans-unit id="breadcrumb.link_answers"&gt;
+                &lt;source&gt;breadcrumb.link_answers&lt;/source&gt;
+                &lt;target&gt;Respuestas&lt;/target&gt;
+            &lt;/trans-unit&gt;</v>
+      </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>23</v>
       </c>
       <c r="B6" t="s">
         <v>25</v>
       </c>
+      <c r="J6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">            &lt;trans-unit id="areas"&gt;
+                &lt;source&gt;areas&lt;/source&gt;
+                &lt;target&gt;Areas&lt;/target&gt;
+            &lt;/trans-unit&gt;</v>
+      </c>
+      <c r="K6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">            &lt;trans-unit id="title_areas"&gt;
+                &lt;source&gt;title_areas&lt;/source&gt;
+                &lt;target&gt;Areas&lt;/target&gt;
+            &lt;/trans-unit&gt;</v>
+      </c>
+      <c r="L6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">            &lt;trans-unit id="label_areas"&gt;
+                &lt;source&gt;label_areas&lt;/source&gt;
+                &lt;target&gt;Areas&lt;/target&gt;
+            &lt;/trans-unit&gt;</v>
+      </c>
+      <c r="M6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">            &lt;trans-unit id="user_form.label_areas"&gt;
+                &lt;source&gt;user_form.label_areas&lt;/source&gt;
+                &lt;target&gt;Areas&lt;/target&gt;
+            &lt;/trans-unit&gt;</v>
+      </c>
+      <c r="N6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">            &lt;trans-unit id="form.label_areas"&gt;
+                &lt;source&gt;form.label_areas&lt;/source&gt;
+                &lt;target&gt;Areas&lt;/target&gt;
+            &lt;/trans-unit&gt;</v>
+      </c>
+      <c r="O6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">            &lt;trans-unit id="filter.label_areas"&gt;
+                &lt;source&gt;filter.label_areas&lt;/source&gt;
+                &lt;target&gt;Areas&lt;/target&gt;
+            &lt;/trans-unit&gt;</v>
+      </c>
+      <c r="P6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">            &lt;trans-unit id="list.label_areas"&gt;
+                &lt;source&gt;list.label_areas&lt;/source&gt;
+                &lt;target&gt;Areas&lt;/target&gt;
+            &lt;/trans-unit&gt;</v>
+      </c>
+      <c r="Q6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">            &lt;trans-unit id="field.label_areas"&gt;
+                &lt;source&gt;field.label_areas&lt;/source&gt;
+                &lt;target&gt;Areas&lt;/target&gt;
+            &lt;/trans-unit&gt;</v>
+      </c>
+      <c r="R6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">            &lt;trans-unit id="show.label_areas"&gt;
+                &lt;source&gt;show.label_areas&lt;/source&gt;
+                &lt;target&gt;Areas&lt;/target&gt;
+            &lt;/trans-unit&gt;</v>
+      </c>
+      <c r="S6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">            &lt;trans-unit id="breadcrumb.link_areas"&gt;
+                &lt;source&gt;breadcrumb.link_areas&lt;/source&gt;
+                &lt;target&gt;Areas&lt;/target&gt;
+            &lt;/trans-unit&gt;</v>
+      </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>24</v>
       </c>
       <c r="B7" t="s">
         <v>26</v>
       </c>
+      <c r="J7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">            &lt;trans-unit id="groups"&gt;
+                &lt;source&gt;groups&lt;/source&gt;
+                &lt;target&gt;Grupos&lt;/target&gt;
+            &lt;/trans-unit&gt;</v>
+      </c>
+      <c r="K7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">            &lt;trans-unit id="title_groups"&gt;
+                &lt;source&gt;title_groups&lt;/source&gt;
+                &lt;target&gt;Grupos&lt;/target&gt;
+            &lt;/trans-unit&gt;</v>
+      </c>
+      <c r="L7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">            &lt;trans-unit id="label_groups"&gt;
+                &lt;source&gt;label_groups&lt;/source&gt;
+                &lt;target&gt;Grupos&lt;/target&gt;
+            &lt;/trans-unit&gt;</v>
+      </c>
+      <c r="M7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">            &lt;trans-unit id="user_form.label_groups"&gt;
+                &lt;source&gt;user_form.label_groups&lt;/source&gt;
+                &lt;target&gt;Grupos&lt;/target&gt;
+            &lt;/trans-unit&gt;</v>
+      </c>
+      <c r="N7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">            &lt;trans-unit id="form.label_groups"&gt;
+                &lt;source&gt;form.label_groups&lt;/source&gt;
+                &lt;target&gt;Grupos&lt;/target&gt;
+            &lt;/trans-unit&gt;</v>
+      </c>
+      <c r="O7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">            &lt;trans-unit id="filter.label_groups"&gt;
+                &lt;source&gt;filter.label_groups&lt;/source&gt;
+                &lt;target&gt;Grupos&lt;/target&gt;
+            &lt;/trans-unit&gt;</v>
+      </c>
+      <c r="P7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">            &lt;trans-unit id="list.label_groups"&gt;
+                &lt;source&gt;list.label_groups&lt;/source&gt;
+                &lt;target&gt;Grupos&lt;/target&gt;
+            &lt;/trans-unit&gt;</v>
+      </c>
+      <c r="Q7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">            &lt;trans-unit id="field.label_groups"&gt;
+                &lt;source&gt;field.label_groups&lt;/source&gt;
+                &lt;target&gt;Grupos&lt;/target&gt;
+            &lt;/trans-unit&gt;</v>
+      </c>
+      <c r="R7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">            &lt;trans-unit id="show.label_groups"&gt;
+                &lt;source&gt;show.label_groups&lt;/source&gt;
+                &lt;target&gt;Grupos&lt;/target&gt;
+            &lt;/trans-unit&gt;</v>
+      </c>
+      <c r="S7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">            &lt;trans-unit id="breadcrumb.link_groups"&gt;
+                &lt;source&gt;breadcrumb.link_groups&lt;/source&gt;
+                &lt;target&gt;Grupos&lt;/target&gt;
+            &lt;/trans-unit&gt;</v>
+      </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>27</v>
       </c>
       <c r="B8" t="s">
         <v>28</v>
+      </c>
+      <c r="J8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">            &lt;trans-unit id="user_limit"&gt;
+                &lt;source&gt;user_limit&lt;/source&gt;
+                &lt;target&gt;Restricción Usuarios&lt;/target&gt;
+            &lt;/trans-unit&gt;</v>
+      </c>
+      <c r="K8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">            &lt;trans-unit id="title_user_limit"&gt;
+                &lt;source&gt;title_user_limit&lt;/source&gt;
+                &lt;target&gt;Restricción Usuarios&lt;/target&gt;
+            &lt;/trans-unit&gt;</v>
+      </c>
+      <c r="L8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">            &lt;trans-unit id="label_user_limit"&gt;
+                &lt;source&gt;label_user_limit&lt;/source&gt;
+                &lt;target&gt;Restricción Usuarios&lt;/target&gt;
+            &lt;/trans-unit&gt;</v>
+      </c>
+      <c r="M8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">            &lt;trans-unit id="user_form.label_user_limit"&gt;
+                &lt;source&gt;user_form.label_user_limit&lt;/source&gt;
+                &lt;target&gt;Restricción Usuarios&lt;/target&gt;
+            &lt;/trans-unit&gt;</v>
+      </c>
+      <c r="N8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">            &lt;trans-unit id="form.label_user_limit"&gt;
+                &lt;source&gt;form.label_user_limit&lt;/source&gt;
+                &lt;target&gt;Restricción Usuarios&lt;/target&gt;
+            &lt;/trans-unit&gt;</v>
+      </c>
+      <c r="O8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">            &lt;trans-unit id="filter.label_user_limit"&gt;
+                &lt;source&gt;filter.label_user_limit&lt;/source&gt;
+                &lt;target&gt;Restricción Usuarios&lt;/target&gt;
+            &lt;/trans-unit&gt;</v>
+      </c>
+      <c r="P8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">            &lt;trans-unit id="list.label_user_limit"&gt;
+                &lt;source&gt;list.label_user_limit&lt;/source&gt;
+                &lt;target&gt;Restricción Usuarios&lt;/target&gt;
+            &lt;/trans-unit&gt;</v>
+      </c>
+      <c r="Q8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">            &lt;trans-unit id="field.label_user_limit"&gt;
+                &lt;source&gt;field.label_user_limit&lt;/source&gt;
+                &lt;target&gt;Restricción Usuarios&lt;/target&gt;
+            &lt;/trans-unit&gt;</v>
+      </c>
+      <c r="R8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">            &lt;trans-unit id="show.label_user_limit"&gt;
+                &lt;source&gt;show.label_user_limit&lt;/source&gt;
+                &lt;target&gt;Restricción Usuarios&lt;/target&gt;
+            &lt;/trans-unit&gt;</v>
+      </c>
+      <c r="S8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">            &lt;trans-unit id="breadcrumb.link_user_limit"&gt;
+                &lt;source&gt;breadcrumb.link_user_limit&lt;/source&gt;
+                &lt;target&gt;Restricción Usuarios&lt;/target&gt;
+            &lt;/trans-unit&gt;</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>